<commit_message>
Lab1, finalizando el laboratorio 1, subiendo tema 2 y tema 3
</commit_message>
<xml_diff>
--- a/Lab1_Procesos/datos_mediciones.xlsx
+++ b/Lab1_Procesos/datos_mediciones.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Unidad</t>
   </si>
@@ -60,6 +60,12 @@
       </rPr>
       <t>). El tiempo "real" fue el medido.</t>
     </r>
+  </si>
+  <si>
+    <t>Laboratorio</t>
+  </si>
+  <si>
+    <t>Lab1: Procesos</t>
   </si>
 </sst>
 </file>
@@ -394,45 +400,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>51.012999999999998</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>